<commit_message>
Actualizar catálogo y corrección de workflow (PowerShell fix)
</commit_message>
<xml_diff>
--- a/Coleccion de minerales.xlsx
+++ b/Coleccion de minerales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascual\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FFB044-EB8C-4A05-854F-EE3A4499012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0D9AF9-33F8-4D0F-A027-51D18613CF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="540">
   <si>
     <t>Mineral</t>
   </si>
@@ -824,9 +824,6 @@
   </si>
   <si>
     <t>81x42x29</t>
-  </si>
-  <si>
-    <t>Ejemplar de malaquita de hábito botroidal, con crecimientos compactos y relieve bien definido, característico de los yacimientos cupríferos del Cinturón del Cobre de la República Democrática del Congo.</t>
   </si>
   <si>
     <t>Adquirido en Feria de Minerales de Cártama 2024</t>
@@ -1753,6 +1750,12 @@
   </si>
   <si>
     <t>Masa densa de cristales de azufre con un hábito euhedral a subhedral. Los cristales son translúcidos y muestran caras brillantes con un brillo resinoso característico. La formación en drusa cubre gran parte de la matriz. Color amarillo "canario" o amarillo limón intenso, extremadamente puro.</t>
+  </si>
+  <si>
+    <t>Libethenita</t>
+  </si>
+  <si>
+    <t>Matriz de roca con incrustaciones de Libethenita que aparecen como pequeños cristales verdes más oscuros y vítreos. Agregados botroidales (en forma de racimo de uvas) de Malaquita. Los nódulos presentan un color verde oscuro profundo y un brillo sedoso a aterciopelado. Conjunto bien equilibrado sobre matriz, con un crecimiento natural muy estético.</t>
   </si>
 </sst>
 </file>
@@ -2167,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="Y69" sqref="Y69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2199,7 +2202,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2211,37 +2214,37 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>346</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>444</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>3</v>
@@ -2250,16 +2253,16 @@
         <v>4</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>348</v>
-      </c>
       <c r="T1" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>5</v>
@@ -2268,10 +2271,10 @@
         <v>6</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>7</v>
@@ -2279,34 +2282,34 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E2" t="s">
         <v>434</v>
       </c>
-      <c r="E2" t="s">
-        <v>435</v>
-      </c>
       <c r="F2" t="s">
+        <v>392</v>
+      </c>
+      <c r="G2" t="s">
+        <v>391</v>
+      </c>
+      <c r="H2" t="s">
         <v>393</v>
       </c>
-      <c r="G2" t="s">
-        <v>392</v>
-      </c>
-      <c r="H2" t="s">
-        <v>394</v>
-      </c>
       <c r="I2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M2" t="s">
         <v>11</v>
@@ -2321,10 +2324,10 @@
         <v>10</v>
       </c>
       <c r="R2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S2" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V2" t="s">
         <v>12</v>
@@ -2344,34 +2347,34 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H3" t="s">
+        <v>394</v>
+      </c>
+      <c r="I3" t="s">
         <v>396</v>
       </c>
-      <c r="H3" t="s">
-        <v>395</v>
-      </c>
-      <c r="I3" t="s">
-        <v>397</v>
-      </c>
       <c r="J3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M3" t="s">
         <v>18</v>
@@ -2386,10 +2389,10 @@
         <v>17</v>
       </c>
       <c r="R3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V3" t="s">
         <v>19</v>
@@ -2406,34 +2409,34 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E4" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M4" t="s">
         <v>22</v>
@@ -2448,10 +2451,10 @@
         <v>21</v>
       </c>
       <c r="R4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V4" t="s">
         <v>23</v>
@@ -2471,37 +2474,37 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F5" t="s">
+        <v>399</v>
+      </c>
+      <c r="G5" t="s">
         <v>400</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>401</v>
       </c>
-      <c r="H5" t="s">
-        <v>402</v>
-      </c>
       <c r="I5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M5" t="s">
         <v>27</v>
@@ -2516,10 +2519,10 @@
         <v>17</v>
       </c>
       <c r="R5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V5" t="s">
         <v>28</v>
@@ -2536,7 +2539,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -2545,22 +2548,22 @@
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F6" t="s">
+        <v>399</v>
+      </c>
+      <c r="G6" t="s">
         <v>400</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>401</v>
       </c>
-      <c r="H6" t="s">
-        <v>402</v>
-      </c>
       <c r="K6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M6" t="s">
         <v>31</v>
@@ -2575,10 +2578,10 @@
         <v>17</v>
       </c>
       <c r="R6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V6" t="s">
         <v>32</v>
@@ -2595,7 +2598,7 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -2604,28 +2607,28 @@
         <v>34</v>
       </c>
       <c r="E7" t="s">
+        <v>402</v>
+      </c>
+      <c r="F7" t="s">
+        <v>356</v>
+      </c>
+      <c r="G7" t="s">
         <v>403</v>
       </c>
-      <c r="F7" t="s">
-        <v>357</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>404</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>405</v>
       </c>
-      <c r="I7" t="s">
-        <v>406</v>
-      </c>
       <c r="J7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M7" t="s">
         <v>36</v>
@@ -2640,10 +2643,10 @@
         <v>17</v>
       </c>
       <c r="R7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V7" t="s">
         <v>37</v>
@@ -2663,37 +2666,37 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B8" t="s">
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E8" t="s">
+        <v>402</v>
+      </c>
+      <c r="F8" t="s">
+        <v>356</v>
+      </c>
+      <c r="G8" t="s">
         <v>403</v>
       </c>
-      <c r="F8" t="s">
-        <v>357</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>404</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>405</v>
       </c>
-      <c r="I8" t="s">
-        <v>406</v>
-      </c>
       <c r="J8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L8" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M8" t="s">
         <v>39</v>
@@ -2702,16 +2705,16 @@
         <v>572</v>
       </c>
       <c r="P8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q8" t="s">
         <v>38</v>
       </c>
       <c r="R8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S8" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V8" t="s">
         <v>40</v>
@@ -2731,37 +2734,37 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B9" t="s">
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E9" t="s">
+        <v>402</v>
+      </c>
+      <c r="F9" t="s">
+        <v>356</v>
+      </c>
+      <c r="G9" t="s">
         <v>403</v>
       </c>
-      <c r="F9" t="s">
-        <v>357</v>
-      </c>
-      <c r="G9" t="s">
-        <v>404</v>
-      </c>
       <c r="H9" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M9" t="s">
         <v>43</v>
@@ -2770,16 +2773,16 @@
         <v>81</v>
       </c>
       <c r="P9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q9" t="s">
         <v>42</v>
       </c>
       <c r="R9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V9" t="s">
         <v>44</v>
@@ -2799,31 +2802,31 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F10" t="s">
+        <v>408</v>
+      </c>
+      <c r="G10" t="s">
         <v>407</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>409</v>
       </c>
-      <c r="G10" t="s">
-        <v>408</v>
-      </c>
-      <c r="I10" t="s">
-        <v>410</v>
-      </c>
       <c r="J10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M10" t="s">
         <v>47</v>
@@ -2838,10 +2841,10 @@
         <v>17</v>
       </c>
       <c r="R10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V10" t="s">
         <v>48</v>
@@ -2858,7 +2861,7 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B11" t="s">
         <v>49</v>
@@ -2867,22 +2870,22 @@
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I11" t="s">
+        <v>411</v>
+      </c>
+      <c r="J11" t="s">
         <v>412</v>
       </c>
-      <c r="J11" t="s">
-        <v>413</v>
-      </c>
       <c r="L11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M11" t="s">
         <v>52</v>
@@ -2891,16 +2894,16 @@
         <v>204</v>
       </c>
       <c r="P11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q11" t="s">
         <v>51</v>
       </c>
       <c r="R11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S11" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V11" t="s">
         <v>53</v>
@@ -2920,7 +2923,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B12" t="s">
         <v>54</v>
@@ -2929,28 +2932,28 @@
         <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I12" t="s">
+        <v>386</v>
+      </c>
+      <c r="J12" t="s">
         <v>387</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>388</v>
       </c>
-      <c r="K12" t="s">
-        <v>389</v>
-      </c>
       <c r="L12" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M12" t="s">
         <v>56</v>
@@ -2959,16 +2962,16 @@
         <v>500</v>
       </c>
       <c r="P12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q12" t="s">
         <v>38</v>
       </c>
       <c r="R12" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V12" t="s">
         <v>57</v>
@@ -2988,34 +2991,34 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D13" t="s">
         <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H13" t="s">
+        <v>415</v>
+      </c>
+      <c r="I13" t="s">
         <v>416</v>
       </c>
-      <c r="I13" t="s">
-        <v>417</v>
-      </c>
       <c r="L13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M13" t="s">
         <v>60</v>
@@ -3024,16 +3027,16 @@
         <v>550</v>
       </c>
       <c r="P13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q13" t="s">
         <v>21</v>
       </c>
       <c r="R13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S13" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V13" t="s">
         <v>61</v>
@@ -3053,7 +3056,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B14" t="s">
         <v>54</v>
@@ -3062,28 +3065,28 @@
         <v>62</v>
       </c>
       <c r="E14" t="s">
+        <v>384</v>
+      </c>
+      <c r="F14" t="s">
+        <v>414</v>
+      </c>
+      <c r="G14" t="s">
+        <v>395</v>
+      </c>
+      <c r="H14" t="s">
+        <v>413</v>
+      </c>
+      <c r="I14" t="s">
+        <v>382</v>
+      </c>
+      <c r="J14" t="s">
+        <v>383</v>
+      </c>
+      <c r="K14" t="s">
         <v>385</v>
       </c>
-      <c r="F14" t="s">
-        <v>415</v>
-      </c>
-      <c r="G14" t="s">
-        <v>396</v>
-      </c>
-      <c r="H14" t="s">
-        <v>414</v>
-      </c>
-      <c r="I14" t="s">
-        <v>383</v>
-      </c>
-      <c r="J14" t="s">
-        <v>384</v>
-      </c>
-      <c r="K14" t="s">
-        <v>386</v>
-      </c>
       <c r="L14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M14" t="s">
         <v>64</v>
@@ -3098,13 +3101,13 @@
         <v>10</v>
       </c>
       <c r="R14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="W14" t="s">
         <v>13</v>
@@ -3121,37 +3124,37 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B15" t="s">
         <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D15" t="s">
         <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H15" t="s">
+        <v>417</v>
+      </c>
+      <c r="I15" t="s">
         <v>418</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>419</v>
       </c>
-      <c r="J15" t="s">
-        <v>420</v>
-      </c>
       <c r="L15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M15" t="s">
         <v>68</v>
@@ -3160,16 +3163,16 @@
         <v>207</v>
       </c>
       <c r="P15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q15" t="s">
         <v>38</v>
       </c>
       <c r="R15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S15" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V15" t="s">
         <v>69</v>
@@ -3189,22 +3192,22 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B16" t="s">
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F16" t="s">
+        <v>420</v>
+      </c>
+      <c r="I16" t="s">
         <v>421</v>
       </c>
-      <c r="I16" t="s">
-        <v>422</v>
-      </c>
       <c r="L16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M16" t="s">
         <v>72</v>
@@ -3219,10 +3222,10 @@
         <v>17</v>
       </c>
       <c r="R16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S16" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V16" t="s">
         <v>73</v>
@@ -3242,34 +3245,34 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F17" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I17" t="s">
+        <v>362</v>
+      </c>
+      <c r="J17" t="s">
         <v>363</v>
       </c>
-      <c r="J17" t="s">
-        <v>364</v>
-      </c>
       <c r="L17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M17" t="s">
         <v>76</v>
@@ -3287,10 +3290,10 @@
         <v>21</v>
       </c>
       <c r="R17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S17" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="V17" t="s">
         <v>78</v>
@@ -3310,7 +3313,7 @@
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B18" t="s">
         <v>79</v>
@@ -3319,25 +3322,25 @@
         <v>80</v>
       </c>
       <c r="E18" t="s">
+        <v>423</v>
+      </c>
+      <c r="F18" t="s">
+        <v>356</v>
+      </c>
+      <c r="G18" t="s">
         <v>424</v>
       </c>
-      <c r="F18" t="s">
-        <v>357</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>425</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>426</v>
       </c>
-      <c r="I18" t="s">
-        <v>427</v>
-      </c>
       <c r="J18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M18" t="s">
         <v>82</v>
@@ -3352,10 +3355,10 @@
         <v>42</v>
       </c>
       <c r="R18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S18" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V18" t="s">
         <v>83</v>
@@ -3375,7 +3378,7 @@
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B19" t="s">
         <v>84</v>
@@ -3387,25 +3390,25 @@
         <v>86</v>
       </c>
       <c r="E19" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F19" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H19" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M19" t="s">
         <v>89</v>
@@ -3420,10 +3423,10 @@
         <v>88</v>
       </c>
       <c r="R19" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S19" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V19" t="s">
         <v>90</v>
@@ -3443,7 +3446,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B20" t="s">
         <v>92</v>
@@ -3452,22 +3455,22 @@
         <v>93</v>
       </c>
       <c r="E20" t="s">
+        <v>374</v>
+      </c>
+      <c r="F20" t="s">
+        <v>376</v>
+      </c>
+      <c r="G20" t="s">
+        <v>446</v>
+      </c>
+      <c r="H20" t="s">
         <v>375</v>
       </c>
-      <c r="F20" t="s">
-        <v>377</v>
-      </c>
-      <c r="G20" t="s">
-        <v>447</v>
-      </c>
-      <c r="H20" t="s">
-        <v>376</v>
-      </c>
       <c r="J20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M20" t="s">
         <v>95</v>
@@ -3482,10 +3485,10 @@
         <v>17</v>
       </c>
       <c r="R20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="V20" t="s">
         <v>96</v>
@@ -3505,7 +3508,7 @@
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B21" t="s">
         <v>67</v>
@@ -3514,25 +3517,25 @@
         <v>97</v>
       </c>
       <c r="E21" t="s">
+        <v>428</v>
+      </c>
+      <c r="F21" t="s">
+        <v>414</v>
+      </c>
+      <c r="G21" t="s">
+        <v>400</v>
+      </c>
+      <c r="H21" t="s">
+        <v>490</v>
+      </c>
+      <c r="I21" t="s">
         <v>429</v>
       </c>
-      <c r="F21" t="s">
-        <v>415</v>
-      </c>
-      <c r="G21" t="s">
-        <v>401</v>
-      </c>
-      <c r="H21" t="s">
-        <v>491</v>
-      </c>
-      <c r="I21" t="s">
-        <v>430</v>
-      </c>
       <c r="J21" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M21" t="s">
         <v>99</v>
@@ -3541,16 +3544,16 @@
         <v>414</v>
       </c>
       <c r="P21" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q21" t="s">
         <v>98</v>
       </c>
       <c r="R21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S21" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V21" t="s">
         <v>100</v>
@@ -3570,7 +3573,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B22" t="s">
         <v>67</v>
@@ -3579,25 +3582,25 @@
         <v>101</v>
       </c>
       <c r="E22" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I22" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J22" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M22" t="s">
         <v>103</v>
@@ -3612,10 +3615,10 @@
         <v>51</v>
       </c>
       <c r="R22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S22" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V22" t="s">
         <v>104</v>
@@ -3635,7 +3638,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B23" t="s">
         <v>67</v>
@@ -3644,25 +3647,25 @@
         <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G23" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H23" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I23" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="L23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M23" t="s">
         <v>106</v>
@@ -3677,10 +3680,10 @@
         <v>51</v>
       </c>
       <c r="R23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V23" t="s">
         <v>107</v>
@@ -3700,37 +3703,37 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B24" t="s">
         <v>108</v>
       </c>
       <c r="C24" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D24" t="s">
         <v>67</v>
       </c>
       <c r="E24" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G24" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H24" t="s">
+        <v>444</v>
+      </c>
+      <c r="I24" t="s">
         <v>445</v>
       </c>
-      <c r="I24" t="s">
-        <v>446</v>
-      </c>
       <c r="J24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M24" t="s">
         <v>111</v>
@@ -3748,10 +3751,10 @@
         <v>110</v>
       </c>
       <c r="R24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V24" t="s">
         <v>113</v>
@@ -3771,37 +3774,37 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B25" t="s">
         <v>115</v>
       </c>
       <c r="C25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G25" t="s">
+        <v>446</v>
+      </c>
+      <c r="H25" t="s">
         <v>447</v>
       </c>
-      <c r="H25" t="s">
-        <v>448</v>
-      </c>
       <c r="I25" t="s">
+        <v>377</v>
+      </c>
+      <c r="J25" t="s">
+        <v>379</v>
+      </c>
+      <c r="K25" t="s">
         <v>378</v>
       </c>
-      <c r="J25" t="s">
-        <v>380</v>
-      </c>
-      <c r="K25" t="s">
-        <v>379</v>
-      </c>
       <c r="L25" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M25" t="s">
         <v>118</v>
@@ -3816,10 +3819,10 @@
         <v>117</v>
       </c>
       <c r="R25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V25" t="s">
         <v>119</v>
@@ -3839,7 +3842,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B26" t="s">
         <v>120</v>
@@ -3848,28 +3851,28 @@
         <v>121</v>
       </c>
       <c r="E26" t="s">
+        <v>448</v>
+      </c>
+      <c r="F26" t="s">
+        <v>356</v>
+      </c>
+      <c r="G26" t="s">
         <v>449</v>
       </c>
-      <c r="F26" t="s">
-        <v>357</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
+        <v>479</v>
+      </c>
+      <c r="I26" t="s">
         <v>450</v>
       </c>
-      <c r="H26" t="s">
-        <v>480</v>
-      </c>
-      <c r="I26" t="s">
-        <v>451</v>
-      </c>
       <c r="J26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="M26" t="s">
         <v>123</v>
@@ -3884,10 +3887,10 @@
         <v>17</v>
       </c>
       <c r="R26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V26" t="s">
         <v>124</v>
@@ -3907,7 +3910,7 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B27" t="s">
         <v>120</v>
@@ -3916,28 +3919,28 @@
         <v>125</v>
       </c>
       <c r="E27" t="s">
+        <v>448</v>
+      </c>
+      <c r="F27" t="s">
+        <v>356</v>
+      </c>
+      <c r="G27" t="s">
         <v>449</v>
       </c>
-      <c r="F27" t="s">
-        <v>357</v>
-      </c>
-      <c r="G27" t="s">
-        <v>450</v>
-      </c>
       <c r="H27" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I27" t="s">
+        <v>452</v>
+      </c>
+      <c r="J27" t="s">
+        <v>354</v>
+      </c>
+      <c r="K27" t="s">
         <v>453</v>
       </c>
-      <c r="J27" t="s">
-        <v>355</v>
-      </c>
-      <c r="K27" t="s">
-        <v>454</v>
-      </c>
       <c r="L27" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M27" t="s">
         <v>126</v>
@@ -3952,10 +3955,10 @@
         <v>17</v>
       </c>
       <c r="R27" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S27" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V27" t="s">
         <v>127</v>
@@ -3972,7 +3975,7 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B28" t="s">
         <v>67</v>
@@ -3984,25 +3987,25 @@
         <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G28" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J28" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L28" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M28" t="s">
         <v>131</v>
@@ -4017,10 +4020,10 @@
         <v>38</v>
       </c>
       <c r="R28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V28" t="s">
         <v>132</v>
@@ -4040,7 +4043,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B29" t="s">
         <v>67</v>
@@ -4049,25 +4052,25 @@
         <v>133</v>
       </c>
       <c r="E29" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H29" t="s">
+        <v>454</v>
+      </c>
+      <c r="I29" t="s">
         <v>455</v>
       </c>
-      <c r="I29" t="s">
-        <v>456</v>
-      </c>
       <c r="J29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L29" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M29" t="s">
         <v>136</v>
@@ -4082,10 +4085,10 @@
         <v>135</v>
       </c>
       <c r="R29" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S29" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V29" t="s">
         <v>137</v>
@@ -4105,34 +4108,34 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B30" t="s">
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E30" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G30" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H30" t="s">
+        <v>456</v>
+      </c>
+      <c r="I30" t="s">
         <v>457</v>
       </c>
-      <c r="I30" t="s">
-        <v>458</v>
-      </c>
       <c r="J30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M30" t="s">
         <v>138</v>
@@ -4141,16 +4144,16 @@
         <v>160</v>
       </c>
       <c r="P30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q30" t="s">
         <v>21</v>
       </c>
       <c r="R30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V30" t="s">
         <v>139</v>
@@ -4170,7 +4173,7 @@
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
@@ -4179,25 +4182,25 @@
         <v>128</v>
       </c>
       <c r="E31" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H31" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K31" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M31" t="s">
         <v>140</v>
@@ -4206,16 +4209,16 @@
         <v>125</v>
       </c>
       <c r="P31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q31" t="s">
         <v>17</v>
       </c>
       <c r="R31" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S31" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V31" t="s">
         <v>141</v>
@@ -4232,7 +4235,7 @@
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B32" t="s">
         <v>33</v>
@@ -4241,28 +4244,28 @@
         <v>34</v>
       </c>
       <c r="E32" t="s">
+        <v>402</v>
+      </c>
+      <c r="F32" t="s">
+        <v>356</v>
+      </c>
+      <c r="G32" t="s">
         <v>403</v>
       </c>
-      <c r="F32" t="s">
-        <v>357</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>404</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>405</v>
       </c>
-      <c r="I32" t="s">
-        <v>406</v>
-      </c>
       <c r="J32" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K32" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L32" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M32" t="s">
         <v>142</v>
@@ -4277,10 +4280,10 @@
         <v>17</v>
       </c>
       <c r="R32" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V32" t="s">
         <v>143</v>
@@ -4297,7 +4300,7 @@
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B33" t="s">
         <v>92</v>
@@ -4306,25 +4309,25 @@
         <v>93</v>
       </c>
       <c r="E33" t="s">
+        <v>374</v>
+      </c>
+      <c r="F33" t="s">
+        <v>376</v>
+      </c>
+      <c r="G33" t="s">
+        <v>446</v>
+      </c>
+      <c r="H33" t="s">
         <v>375</v>
       </c>
-      <c r="F33" t="s">
-        <v>377</v>
-      </c>
-      <c r="G33" t="s">
-        <v>447</v>
-      </c>
-      <c r="H33" t="s">
-        <v>376</v>
-      </c>
       <c r="J33" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L33" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M33" t="s">
         <v>144</v>
@@ -4339,10 +4342,10 @@
         <v>17</v>
       </c>
       <c r="R33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S33" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V33" t="s">
         <v>145</v>
@@ -4362,7 +4365,7 @@
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B34" t="s">
         <v>120</v>
@@ -4371,28 +4374,28 @@
         <v>125</v>
       </c>
       <c r="E34" t="s">
+        <v>448</v>
+      </c>
+      <c r="F34" t="s">
+        <v>356</v>
+      </c>
+      <c r="G34" t="s">
         <v>449</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" t="s">
+        <v>479</v>
+      </c>
+      <c r="I34" t="s">
+        <v>353</v>
+      </c>
+      <c r="J34" t="s">
+        <v>354</v>
+      </c>
+      <c r="K34" t="s">
         <v>357</v>
       </c>
-      <c r="G34" t="s">
-        <v>450</v>
-      </c>
-      <c r="H34" t="s">
-        <v>480</v>
-      </c>
-      <c r="I34" t="s">
-        <v>354</v>
-      </c>
-      <c r="J34" t="s">
-        <v>355</v>
-      </c>
-      <c r="K34" t="s">
-        <v>358</v>
-      </c>
       <c r="L34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M34" t="s">
         <v>148</v>
@@ -4407,10 +4410,10 @@
         <v>17</v>
       </c>
       <c r="R34" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S34" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V34" t="s">
         <v>149</v>
@@ -4430,34 +4433,34 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B35" t="s">
         <v>150</v>
       </c>
       <c r="C35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E35" t="s">
+        <v>461</v>
+      </c>
+      <c r="F35" t="s">
         <v>462</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
+        <v>407</v>
+      </c>
+      <c r="H35" t="s">
         <v>463</v>
       </c>
-      <c r="G35" t="s">
-        <v>408</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>464</v>
       </c>
-      <c r="I35" t="s">
-        <v>465</v>
-      </c>
       <c r="K35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L35" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M35" t="s">
         <v>151</v>
@@ -4466,16 +4469,16 @@
         <v>565</v>
       </c>
       <c r="P35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q35" t="s">
         <v>88</v>
       </c>
       <c r="R35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V35" t="s">
         <v>152</v>
@@ -4495,37 +4498,37 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B36" t="s">
         <v>153</v>
       </c>
       <c r="C36" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E36" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F36" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H36" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I36" t="s">
+        <v>365</v>
+      </c>
+      <c r="J36" t="s">
         <v>366</v>
       </c>
-      <c r="J36" t="s">
-        <v>367</v>
-      </c>
       <c r="K36" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L36" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M36" t="s">
         <v>155</v>
@@ -4540,10 +4543,10 @@
         <v>88</v>
       </c>
       <c r="R36" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S36" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V36" t="s">
         <v>156</v>
@@ -4563,7 +4566,7 @@
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B37" t="s">
         <v>92</v>
@@ -4572,22 +4575,22 @@
         <v>157</v>
       </c>
       <c r="E37" t="s">
+        <v>374</v>
+      </c>
+      <c r="F37" t="s">
+        <v>376</v>
+      </c>
+      <c r="G37" t="s">
+        <v>446</v>
+      </c>
+      <c r="H37" t="s">
         <v>375</v>
       </c>
-      <c r="F37" t="s">
-        <v>377</v>
-      </c>
-      <c r="G37" t="s">
-        <v>447</v>
-      </c>
-      <c r="H37" t="s">
-        <v>376</v>
-      </c>
       <c r="K37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L37" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M37" t="s">
         <v>158</v>
@@ -4602,10 +4605,10 @@
         <v>21</v>
       </c>
       <c r="R37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S37" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V37" t="s">
         <v>159</v>
@@ -4625,7 +4628,7 @@
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B38" t="s">
         <v>92</v>
@@ -4634,22 +4637,22 @@
         <v>157</v>
       </c>
       <c r="E38" t="s">
+        <v>374</v>
+      </c>
+      <c r="F38" t="s">
+        <v>376</v>
+      </c>
+      <c r="G38" t="s">
+        <v>446</v>
+      </c>
+      <c r="H38" t="s">
         <v>375</v>
       </c>
-      <c r="F38" t="s">
-        <v>377</v>
-      </c>
-      <c r="G38" t="s">
-        <v>447</v>
-      </c>
-      <c r="H38" t="s">
-        <v>376</v>
-      </c>
       <c r="K38" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L38" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M38" t="s">
         <v>160</v>
@@ -4658,16 +4661,16 @@
         <v>109</v>
       </c>
       <c r="P38" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q38" t="s">
         <v>21</v>
       </c>
       <c r="R38" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V38" t="s">
         <v>161</v>
@@ -4684,7 +4687,7 @@
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B39" t="s">
         <v>92</v>
@@ -4693,22 +4696,22 @@
         <v>157</v>
       </c>
       <c r="E39" t="s">
+        <v>374</v>
+      </c>
+      <c r="F39" t="s">
+        <v>376</v>
+      </c>
+      <c r="G39" t="s">
+        <v>446</v>
+      </c>
+      <c r="H39" t="s">
         <v>375</v>
       </c>
-      <c r="F39" t="s">
-        <v>377</v>
-      </c>
-      <c r="G39" t="s">
-        <v>447</v>
-      </c>
-      <c r="H39" t="s">
-        <v>376</v>
-      </c>
       <c r="K39" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L39" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M39" t="s">
         <v>162</v>
@@ -4717,16 +4720,16 @@
         <v>300</v>
       </c>
       <c r="P39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q39" t="s">
         <v>21</v>
       </c>
       <c r="R39" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V39" t="s">
         <v>163</v>
@@ -4743,7 +4746,7 @@
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B40" t="s">
         <v>92</v>
@@ -4752,22 +4755,22 @@
         <v>157</v>
       </c>
       <c r="E40" t="s">
+        <v>374</v>
+      </c>
+      <c r="F40" t="s">
+        <v>376</v>
+      </c>
+      <c r="G40" t="s">
+        <v>446</v>
+      </c>
+      <c r="H40" t="s">
         <v>375</v>
       </c>
-      <c r="F40" t="s">
-        <v>377</v>
-      </c>
-      <c r="G40" t="s">
-        <v>447</v>
-      </c>
-      <c r="H40" t="s">
-        <v>376</v>
-      </c>
       <c r="K40" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L40" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M40" t="s">
         <v>164</v>
@@ -4776,16 +4779,16 @@
         <v>115</v>
       </c>
       <c r="P40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q40" t="s">
         <v>21</v>
       </c>
       <c r="R40" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V40" t="s">
         <v>165</v>
@@ -4802,34 +4805,34 @@
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B41" t="s">
         <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E41" t="s">
+        <v>466</v>
+      </c>
+      <c r="F41" t="s">
+        <v>392</v>
+      </c>
+      <c r="G41" t="s">
+        <v>407</v>
+      </c>
+      <c r="H41" t="s">
         <v>467</v>
       </c>
-      <c r="F41" t="s">
-        <v>393</v>
-      </c>
-      <c r="G41" t="s">
-        <v>408</v>
-      </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>468</v>
       </c>
-      <c r="I41" t="s">
-        <v>469</v>
-      </c>
       <c r="K41" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L41" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M41" t="s">
         <v>167</v>
@@ -4838,16 +4841,16 @@
         <v>819</v>
       </c>
       <c r="P41" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q41" t="s">
         <v>88</v>
       </c>
       <c r="R41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V41" t="s">
         <v>168</v>
@@ -4867,37 +4870,37 @@
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B42" t="s">
         <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E42" t="s">
+        <v>469</v>
+      </c>
+      <c r="F42" t="s">
+        <v>392</v>
+      </c>
+      <c r="G42" t="s">
+        <v>446</v>
+      </c>
+      <c r="H42" t="s">
         <v>470</v>
       </c>
-      <c r="F42" t="s">
-        <v>393</v>
-      </c>
-      <c r="G42" t="s">
-        <v>447</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="I42" t="s">
         <v>471</v>
       </c>
-      <c r="I42" t="s">
-        <v>472</v>
-      </c>
       <c r="J42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K42" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M42" t="s">
         <v>171</v>
@@ -4912,10 +4915,10 @@
         <v>17</v>
       </c>
       <c r="R42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S42" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T42" s="1">
         <v>45199</v>
@@ -4941,34 +4944,34 @@
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B43" t="s">
         <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E43" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F43" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G43" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H43" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I43" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K43" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L43" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M43" t="s">
         <v>175</v>
@@ -4983,10 +4986,10 @@
         <v>17</v>
       </c>
       <c r="R43" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S43" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T43" s="1">
         <v>45199</v>
@@ -5012,37 +5015,37 @@
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B44" t="s">
         <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E44" t="s">
+        <v>402</v>
+      </c>
+      <c r="F44" t="s">
+        <v>356</v>
+      </c>
+      <c r="G44" t="s">
         <v>403</v>
       </c>
-      <c r="F44" t="s">
-        <v>357</v>
-      </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>404</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>405</v>
       </c>
-      <c r="I44" t="s">
-        <v>406</v>
-      </c>
       <c r="J44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L44" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M44" t="s">
         <v>177</v>
@@ -5060,10 +5063,10 @@
         <v>17</v>
       </c>
       <c r="R44" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S44" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T44" s="1">
         <v>45199</v>
@@ -5089,37 +5092,37 @@
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B45" t="s">
         <v>180</v>
       </c>
       <c r="C45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D45" t="s">
         <v>70</v>
       </c>
       <c r="E45" t="s">
+        <v>472</v>
+      </c>
+      <c r="F45" t="s">
+        <v>414</v>
+      </c>
+      <c r="G45" t="s">
+        <v>395</v>
+      </c>
+      <c r="H45" t="s">
         <v>473</v>
       </c>
-      <c r="F45" t="s">
-        <v>415</v>
-      </c>
-      <c r="G45" t="s">
-        <v>396</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>474</v>
       </c>
-      <c r="I45" t="s">
-        <v>475</v>
-      </c>
       <c r="K45" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L45" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M45" t="s">
         <v>182</v>
@@ -5134,10 +5137,10 @@
         <v>17</v>
       </c>
       <c r="R45" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T45" s="1">
         <v>45213</v>
@@ -5163,37 +5166,37 @@
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B46" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C46" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E46" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F46" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G46" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H46" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I46" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J46" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K46" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L46" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M46" t="s">
         <v>187</v>
@@ -5208,10 +5211,10 @@
         <v>186</v>
       </c>
       <c r="R46" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S46" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T46" s="1">
         <v>45215</v>
@@ -5237,7 +5240,7 @@
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B47" t="s">
         <v>67</v>
@@ -5246,22 +5249,22 @@
         <v>128</v>
       </c>
       <c r="E47" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F47" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H47" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K47" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L47" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M47" t="s">
         <v>192</v>
@@ -5276,10 +5279,10 @@
         <v>191</v>
       </c>
       <c r="R47" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S47" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T47" s="1">
         <v>45233</v>
@@ -5305,28 +5308,28 @@
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B48" t="s">
         <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E48" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H48" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="L48" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M48" t="s">
         <v>196</v>
@@ -5341,10 +5344,10 @@
         <v>17</v>
       </c>
       <c r="R48" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S48" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T48" s="1">
         <v>45233</v>
@@ -5370,7 +5373,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B49" t="s">
         <v>67</v>
@@ -5379,28 +5382,28 @@
         <v>105</v>
       </c>
       <c r="E49" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F49" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G49" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H49" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I49" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="J49" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K49" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L49" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M49" t="s">
         <v>199</v>
@@ -5415,10 +5418,10 @@
         <v>198</v>
       </c>
       <c r="R49" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S49" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T49" s="1">
         <v>45236</v>
@@ -5444,7 +5447,7 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B50" t="s">
         <v>120</v>
@@ -5453,25 +5456,25 @@
         <v>125</v>
       </c>
       <c r="E50" t="s">
+        <v>448</v>
+      </c>
+      <c r="F50" t="s">
+        <v>356</v>
+      </c>
+      <c r="G50" t="s">
         <v>449</v>
       </c>
-      <c r="F50" t="s">
-        <v>357</v>
-      </c>
-      <c r="G50" t="s">
-        <v>450</v>
-      </c>
       <c r="H50" t="s">
+        <v>479</v>
+      </c>
+      <c r="I50" t="s">
         <v>480</v>
       </c>
-      <c r="I50" t="s">
-        <v>481</v>
-      </c>
       <c r="J50" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L50" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M50" t="s">
         <v>203</v>
@@ -5486,10 +5489,10 @@
         <v>17</v>
       </c>
       <c r="R50" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S50" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T50" s="1">
         <v>45247</v>
@@ -5515,34 +5518,34 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B51" t="s">
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E51" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F51" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G51" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H51" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I51" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J51" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L51" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M51" t="s">
         <v>206</v>
@@ -5551,16 +5554,16 @@
         <v>3900</v>
       </c>
       <c r="P51" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q51" t="s">
         <v>205</v>
       </c>
       <c r="R51" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S51" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V51" t="s">
         <v>207</v>
@@ -5580,7 +5583,7 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B52" t="s">
         <v>67</v>
@@ -5589,28 +5592,28 @@
         <v>209</v>
       </c>
       <c r="E52" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F52" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G52" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H52" t="s">
+        <v>482</v>
+      </c>
+      <c r="I52" t="s">
         <v>483</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>484</v>
       </c>
-      <c r="J52" t="s">
-        <v>485</v>
-      </c>
       <c r="K52" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L52" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M52" t="s">
         <v>210</v>
@@ -5619,16 +5622,16 @@
         <v>1850</v>
       </c>
       <c r="P52" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q52" t="s">
         <v>205</v>
       </c>
       <c r="R52" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S52" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V52" t="s">
         <v>211</v>
@@ -5648,34 +5651,34 @@
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B53" t="s">
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E53" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F53" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G53" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H53" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I53" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J53" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M53" t="s">
         <v>213</v>
@@ -5684,16 +5687,16 @@
         <v>350</v>
       </c>
       <c r="P53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q53" t="s">
         <v>21</v>
       </c>
       <c r="R53" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V53" t="s">
         <v>214</v>
@@ -5713,7 +5716,7 @@
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B54" t="s">
         <v>67</v>
@@ -5722,25 +5725,25 @@
         <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F54" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G54" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H54" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I54" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="J54" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M54" t="s">
         <v>216</v>
@@ -5749,16 +5752,16 @@
         <v>269</v>
       </c>
       <c r="P54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q54" t="s">
         <v>21</v>
       </c>
       <c r="R54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S54" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="V54" t="s">
         <v>217</v>
@@ -5778,7 +5781,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B55" t="s">
         <v>219</v>
@@ -5790,25 +5793,25 @@
         <v>86</v>
       </c>
       <c r="E55" t="s">
+        <v>487</v>
+      </c>
+      <c r="F55" t="s">
+        <v>399</v>
+      </c>
+      <c r="G55" t="s">
+        <v>407</v>
+      </c>
+      <c r="H55" t="s">
         <v>488</v>
       </c>
-      <c r="F55" t="s">
-        <v>400</v>
-      </c>
-      <c r="G55" t="s">
-        <v>408</v>
-      </c>
-      <c r="H55" t="s">
-        <v>489</v>
-      </c>
       <c r="I55" t="s">
+        <v>368</v>
+      </c>
+      <c r="J55" t="s">
         <v>369</v>
       </c>
-      <c r="J55" t="s">
-        <v>370</v>
-      </c>
       <c r="L55" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M55" t="s">
         <v>221</v>
@@ -5826,10 +5829,10 @@
         <v>88</v>
       </c>
       <c r="R55" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S55" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T55" s="1">
         <v>45267</v>
@@ -5855,37 +5858,37 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B56" t="s">
         <v>224</v>
       </c>
       <c r="C56" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E56" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G56" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H56" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I56" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J56" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L56" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M56" t="s">
         <v>225</v>
@@ -5894,16 +5897,16 @@
         <v>375</v>
       </c>
       <c r="P56" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q56" t="s">
         <v>21</v>
       </c>
       <c r="R56" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S56" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T56" s="1">
         <v>45267</v>
@@ -5929,7 +5932,7 @@
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B57" t="s">
         <v>67</v>
@@ -5938,25 +5941,25 @@
         <v>101</v>
       </c>
       <c r="E57" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F57" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G57" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H57" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I57" t="s">
         <v>121</v>
       </c>
       <c r="J57" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L57" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M57" t="s">
         <v>227</v>
@@ -5965,16 +5968,16 @@
         <v>510</v>
       </c>
       <c r="P57" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q57" t="s">
         <v>51</v>
       </c>
       <c r="R57" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S57" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T57" s="1">
         <v>45267</v>
@@ -6000,7 +6003,7 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B58" t="s">
         <v>67</v>
@@ -6009,28 +6012,28 @@
         <v>229</v>
       </c>
       <c r="E58" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F58" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G58" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H58" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I58" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K58" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L58" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M58" t="s">
         <v>231</v>
@@ -6045,10 +6048,10 @@
         <v>21</v>
       </c>
       <c r="R58" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S58" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T58" s="1">
         <v>45269</v>
@@ -6074,37 +6077,40 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B59" t="s">
+        <v>538</v>
+      </c>
+      <c r="C59" t="s">
+        <v>433</v>
+      </c>
+      <c r="D59" t="s">
         <v>58</v>
       </c>
-      <c r="C59" t="s">
-        <v>434</v>
-      </c>
       <c r="E59" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G59" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H59" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I59" t="s">
+        <v>389</v>
+      </c>
+      <c r="J59" t="s">
         <v>390</v>
       </c>
-      <c r="J59" t="s">
-        <v>391</v>
-      </c>
       <c r="K59" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L59" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M59" t="s">
         <v>236</v>
@@ -6119,10 +6125,10 @@
         <v>235</v>
       </c>
       <c r="R59" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S59" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T59" s="1">
         <v>45571</v>
@@ -6131,10 +6137,10 @@
         <v>60</v>
       </c>
       <c r="V59" t="s">
+        <v>539</v>
+      </c>
+      <c r="W59" t="s">
         <v>237</v>
-      </c>
-      <c r="W59" t="s">
-        <v>238</v>
       </c>
       <c r="X59">
         <v>70</v>
@@ -6148,52 +6154,52 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C60" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D60" t="s">
         <v>58</v>
       </c>
       <c r="E60" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F60" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G60" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H60" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I60" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L60" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O60">
         <v>250</v>
       </c>
       <c r="P60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q60" t="s">
         <v>42</v>
       </c>
       <c r="R60" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S60" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T60" s="1">
         <v>45591</v>
@@ -6202,10 +6208,10 @@
         <v>35</v>
       </c>
       <c r="V60" t="s">
+        <v>241</v>
+      </c>
+      <c r="W60" t="s">
         <v>242</v>
-      </c>
-      <c r="W60" t="s">
-        <v>243</v>
       </c>
       <c r="X60">
         <v>90</v>
@@ -6219,55 +6225,55 @@
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B61" t="s">
         <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E61" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F61" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G61" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H61" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I61" t="s">
+        <v>371</v>
+      </c>
+      <c r="J61" t="s">
         <v>372</v>
       </c>
-      <c r="J61" t="s">
-        <v>373</v>
-      </c>
       <c r="L61" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M61" t="s">
+        <v>244</v>
+      </c>
+      <c r="N61" t="s">
         <v>245</v>
-      </c>
-      <c r="N61" t="s">
-        <v>246</v>
       </c>
       <c r="O61">
         <v>200</v>
       </c>
       <c r="P61" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q61" t="s">
         <v>21</v>
       </c>
       <c r="R61" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S61" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T61" s="1">
         <v>45635</v>
@@ -6276,10 +6282,10 @@
         <v>36</v>
       </c>
       <c r="V61" t="s">
+        <v>246</v>
+      </c>
+      <c r="W61" t="s">
         <v>247</v>
-      </c>
-      <c r="W61" t="s">
-        <v>248</v>
       </c>
       <c r="X61">
         <v>100</v>
@@ -6288,57 +6294,57 @@
         <v>46031</v>
       </c>
       <c r="Z61" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B62" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C62" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D62" t="s">
         <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F62" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G62" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H62" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I62" t="s">
         <v>184</v>
       </c>
       <c r="L62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O62">
         <v>370</v>
       </c>
       <c r="P62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="Q62" t="s">
         <v>51</v>
       </c>
       <c r="R62" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S62" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T62" s="1">
         <v>45646</v>
@@ -6347,10 +6353,10 @@
         <v>50</v>
       </c>
       <c r="V62" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="X62">
         <v>110</v>
@@ -6364,58 +6370,58 @@
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B63" t="s">
         <v>67</v>
       </c>
       <c r="C63" t="s">
+        <v>253</v>
+      </c>
+      <c r="D63" t="s">
         <v>254</v>
       </c>
-      <c r="D63" t="s">
-        <v>255</v>
-      </c>
       <c r="E63" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F63" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G63" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H63" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J63" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K63" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L63" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M63" t="s">
+        <v>256</v>
+      </c>
+      <c r="N63" t="s">
         <v>257</v>
-      </c>
-      <c r="N63" t="s">
-        <v>258</v>
       </c>
       <c r="O63">
         <v>3500</v>
       </c>
       <c r="P63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R63" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S63" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T63" s="1">
         <v>45839</v>
@@ -6424,10 +6430,10 @@
         <v>160</v>
       </c>
       <c r="V63" t="s">
+        <v>258</v>
+      </c>
+      <c r="W63" t="s">
         <v>259</v>
-      </c>
-      <c r="W63" t="s">
-        <v>260</v>
       </c>
       <c r="X63">
         <v>300</v>
@@ -6441,7 +6447,7 @@
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B64" t="s">
         <v>67</v>
@@ -6450,46 +6456,46 @@
         <v>229</v>
       </c>
       <c r="E64" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F64" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H64" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J64" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L64" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M64" t="s">
+        <v>261</v>
+      </c>
+      <c r="N64" t="s">
         <v>262</v>
-      </c>
-      <c r="N64" t="s">
-        <v>263</v>
       </c>
       <c r="O64">
         <v>225</v>
       </c>
       <c r="P64" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q64" t="s">
         <v>21</v>
       </c>
       <c r="R64" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S64" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T64" s="1">
         <v>45996</v>
@@ -6498,10 +6504,10 @@
         <v>75</v>
       </c>
       <c r="V64" t="s">
+        <v>263</v>
+      </c>
+      <c r="W64" t="s">
         <v>264</v>
-      </c>
-      <c r="W64" t="s">
-        <v>265</v>
       </c>
       <c r="X64">
         <v>120</v>
@@ -6515,58 +6521,58 @@
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C65" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D65" t="s">
         <v>33</v>
       </c>
       <c r="E65" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F65" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G65" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H65" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I65" t="s">
+        <v>359</v>
+      </c>
+      <c r="J65" t="s">
         <v>360</v>
       </c>
-      <c r="J65" t="s">
-        <v>361</v>
-      </c>
       <c r="K65" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L65" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O65">
         <v>105</v>
       </c>
       <c r="P65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q65" t="s">
         <v>38</v>
       </c>
       <c r="R65" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S65" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T65" s="1">
         <v>46013</v>
@@ -6575,10 +6581,10 @@
         <v>30</v>
       </c>
       <c r="V65" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="W65" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="X65">
         <v>150</v>
@@ -6592,52 +6598,52 @@
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B66" t="s">
         <v>209</v>
       </c>
       <c r="C66" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E66" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F66" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G66" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H66" t="s">
+        <v>513</v>
+      </c>
+      <c r="I66" t="s">
         <v>514</v>
       </c>
-      <c r="I66" t="s">
+      <c r="K66" t="s">
+        <v>388</v>
+      </c>
+      <c r="L66" t="s">
+        <v>351</v>
+      </c>
+      <c r="M66" t="s">
         <v>515</v>
-      </c>
-      <c r="K66" t="s">
-        <v>389</v>
-      </c>
-      <c r="L66" t="s">
-        <v>352</v>
-      </c>
-      <c r="M66" t="s">
-        <v>516</v>
       </c>
       <c r="O66">
         <v>86</v>
       </c>
       <c r="P66" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q66" t="s">
         <v>17</v>
       </c>
       <c r="R66" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S66" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T66" s="6">
         <v>46041</v>
@@ -6646,10 +6652,10 @@
         <v>0</v>
       </c>
       <c r="V66" t="s">
+        <v>517</v>
+      </c>
+      <c r="W66" t="s">
         <v>518</v>
-      </c>
-      <c r="W66" t="s">
-        <v>519</v>
       </c>
       <c r="X66">
         <v>15</v>
@@ -6663,55 +6669,55 @@
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B67" t="s">
         <v>169</v>
       </c>
       <c r="C67" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E67" t="s">
+        <v>469</v>
+      </c>
+      <c r="F67" t="s">
+        <v>392</v>
+      </c>
+      <c r="G67" t="s">
+        <v>446</v>
+      </c>
+      <c r="H67" t="s">
         <v>470</v>
       </c>
-      <c r="F67" t="s">
-        <v>393</v>
-      </c>
-      <c r="G67" t="s">
-        <v>447</v>
-      </c>
-      <c r="H67" t="s">
-        <v>471</v>
-      </c>
       <c r="I67" t="s">
+        <v>519</v>
+      </c>
+      <c r="J67" t="s">
         <v>520</v>
       </c>
-      <c r="J67" t="s">
+      <c r="K67" t="s">
         <v>521</v>
       </c>
-      <c r="K67" t="s">
+      <c r="L67" t="s">
+        <v>351</v>
+      </c>
+      <c r="M67" t="s">
         <v>522</v>
-      </c>
-      <c r="L67" t="s">
-        <v>352</v>
-      </c>
-      <c r="M67" t="s">
-        <v>523</v>
       </c>
       <c r="O67">
         <v>28</v>
       </c>
       <c r="P67" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="Q67" t="s">
         <v>38</v>
       </c>
       <c r="R67" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S67" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T67" s="6">
         <v>46041</v>
@@ -6720,10 +6726,10 @@
         <v>25</v>
       </c>
       <c r="V67" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="W67" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="X67">
         <v>60</v>
@@ -6737,7 +6743,7 @@
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B68" t="s">
         <v>67</v>
@@ -6746,46 +6752,46 @@
         <v>101</v>
       </c>
       <c r="E68" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F68" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G68" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H68" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I68" t="s">
+        <v>524</v>
+      </c>
+      <c r="J68" t="s">
+        <v>354</v>
+      </c>
+      <c r="K68" t="s">
+        <v>476</v>
+      </c>
+      <c r="L68" t="s">
+        <v>351</v>
+      </c>
+      <c r="M68" t="s">
         <v>525</v>
-      </c>
-      <c r="J68" t="s">
-        <v>355</v>
-      </c>
-      <c r="K68" t="s">
-        <v>477</v>
-      </c>
-      <c r="L68" t="s">
-        <v>352</v>
-      </c>
-      <c r="M68" t="s">
-        <v>526</v>
       </c>
       <c r="O68">
         <v>92</v>
       </c>
       <c r="P68" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="Q68" t="s">
         <v>10</v>
       </c>
       <c r="R68" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S68" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T68" s="6">
         <v>46041</v>
@@ -6794,10 +6800,10 @@
         <v>30</v>
       </c>
       <c r="V68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="W68" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="X68">
         <v>85</v>
@@ -6811,55 +6817,55 @@
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B69" t="s">
+        <v>528</v>
+      </c>
+      <c r="C69" t="s">
+        <v>433</v>
+      </c>
+      <c r="E69" t="s">
         <v>529</v>
       </c>
-      <c r="C69" t="s">
-        <v>434</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
+        <v>392</v>
+      </c>
+      <c r="G69" t="s">
+        <v>424</v>
+      </c>
+      <c r="H69" t="s">
         <v>530</v>
       </c>
-      <c r="F69" t="s">
-        <v>393</v>
-      </c>
-      <c r="G69" t="s">
-        <v>425</v>
-      </c>
-      <c r="H69" t="s">
+      <c r="I69" t="s">
         <v>531</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
+        <v>363</v>
+      </c>
+      <c r="K69" t="s">
         <v>532</v>
       </c>
-      <c r="J69" t="s">
-        <v>364</v>
-      </c>
-      <c r="K69" t="s">
+      <c r="L69" t="s">
+        <v>351</v>
+      </c>
+      <c r="M69" t="s">
         <v>533</v>
-      </c>
-      <c r="L69" t="s">
-        <v>352</v>
-      </c>
-      <c r="M69" t="s">
-        <v>534</v>
       </c>
       <c r="O69">
         <v>160</v>
       </c>
       <c r="P69" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="Q69" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="R69" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S69" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="T69" s="6">
         <v>46041</v>
@@ -6868,10 +6874,10 @@
         <v>60</v>
       </c>
       <c r="V69" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="W69" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="X69">
         <v>150</v>

</xml_diff>